<commit_message>
#fix: sap_connection on start by rust
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -43,6 +43,12 @@
     <t>ABRACADEIRA FF REPARO TUBO DN50 LMIN=150</t>
   </si>
   <si>
+    <t>30001122</t>
+  </si>
+  <si>
+    <t>ABRACADEIRA FF REPARO TUBO DN75 LMIN=150</t>
+  </si>
+  <si>
     <t>30004242</t>
   </si>
   <si>
@@ -299,12 +305,6 @@
   </si>
   <si>
     <t>LUVA CORRER BB ESG DN 300 - JEI</t>
-  </si>
-  <si>
-    <t>30005906</t>
-  </si>
-  <si>
-    <t>LUVA CORRER FF BOLSAS JE2GS DN100</t>
   </si>
   <si>
     <t>30005917</t>
@@ -820,13 +820,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>1.000</v>
+        <v>20.000</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="3">
-        <v>97.58</v>
+        <v>8551.58</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -846,13 +846,13 @@
         <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>19.000</v>
+        <v>1.000</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="3">
-        <v>1798.43</v>
+        <v>97.58</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -872,13 +872,13 @@
         <v>15</v>
       </c>
       <c r="F7" s="2">
-        <v>4.000</v>
+        <v>19.000</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="3">
-        <v>155.83</v>
+        <v>1798.43</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -898,13 +898,13 @@
         <v>17</v>
       </c>
       <c r="F8" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="3">
-        <v>59.98</v>
+        <v>155.83</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -924,13 +924,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>226.62</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -950,13 +950,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
-        <v>225.05</v>
+        <v>226.62</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -976,13 +976,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>10.000</v>
+        <v>5.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>325.39</v>
+        <v>225.05</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1002,13 +1002,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>335.45</v>
+        <v>325.39</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1034,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>62.76</v>
+        <v>335.45</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1054,13 +1054,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>1902.52</v>
+        <v>62.76</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1080,13 +1080,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="2">
-        <v>186.000</v>
+        <v>12.000</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>103932.33</v>
+        <v>1902.52</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1106,13 +1106,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>798.000</v>
+        <v>186.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>7271.36</v>
+        <v>103932.25</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1132,13 +1132,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>30.000</v>
+        <v>797.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>480.88</v>
+        <v>7262.27</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1158,13 +1158,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>1.000</v>
+        <v>30.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>27.05</v>
+        <v>480.88</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1184,13 +1184,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="2">
-        <v>630.000</v>
+        <v>1.000</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>6490.81</v>
+        <v>27.05</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1210,13 +1210,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>2.000</v>
+        <v>630.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>246.82</v>
+        <v>6490.83</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1236,13 +1236,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>281.92</v>
+        <v>246.82</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1262,13 +1262,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>6.000</v>
+        <v>5.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>417.59</v>
+        <v>281.92</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1288,13 +1288,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>130.63</v>
+        <v>417.59</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1314,13 +1314,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>22.000</v>
+        <v>5.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>114.36</v>
+        <v>130.63</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1340,13 +1340,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>14.000</v>
+        <v>22.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>1756.56</v>
+        <v>114.36</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1366,13 +1366,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>2.000</v>
+        <v>14.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>17.76</v>
+        <v>1756.56</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1392,13 +1392,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>50.000</v>
+        <v>1.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>979.54</v>
+        <v>8.88</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1418,13 +1418,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>4.000</v>
+        <v>49.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>227.12</v>
+        <v>959.95</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1444,13 +1444,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>286.67</v>
+        <v>227.12</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1470,13 +1470,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>195.000</v>
+        <v>5.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>1209.63</v>
+        <v>286.67</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1496,13 +1496,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>50.000</v>
+        <v>193.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>545.23</v>
+        <v>1197.23</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1522,13 +1522,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>1591.000</v>
+        <v>50.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>41440.88</v>
+        <v>545.23</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1548,13 +1548,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>183.000</v>
+        <v>1556.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>15549.39</v>
+        <v>40529.20</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1574,13 +1574,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>1026.000</v>
+        <v>181.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>141326.37</v>
+        <v>15379.45</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1600,13 +1600,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>4.000</v>
+        <v>921.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>1412.53</v>
+        <v>126863.14</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1626,13 +1626,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>86.000</v>
+        <v>4.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>3191.52</v>
+        <v>1412.53</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1652,13 +1652,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>38.000</v>
+        <v>82.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>2484.01</v>
+        <v>3043.09</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1678,13 +1678,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>50.000</v>
+        <v>38.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>1647.35</v>
+        <v>2484.01</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1704,13 +1704,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>26.000</v>
+        <v>50.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>877.88</v>
+        <v>1647.35</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1730,13 +1730,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>3839.000</v>
+        <v>26.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>14842.32</v>
+        <v>877.88</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1756,13 +1756,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>2.000</v>
+        <v>3578.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>2173.68</v>
+        <v>13832.96</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1782,13 +1782,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>10582.48</v>
+        <v>2173.68</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1808,13 +1808,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>10490.44</v>
+        <v>10582.47</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1834,13 +1834,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>1650.27</v>
+        <v>10490.44</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1860,13 +1860,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>10.000</v>
+        <v>4.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>14423.65</v>
+        <v>1650.27</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1886,13 +1886,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>353.000</v>
+        <v>10.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>1998.26</v>
+        <v>14423.65</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1912,13 +1912,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>4.000</v>
+        <v>349.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>455.14</v>
+        <v>1975.62</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1938,13 +1938,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>159.15</v>
+        <v>455.14</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2172,13 +2172,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>273.000</v>
+        <v>259.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>5111.93</v>
+        <v>4849.78</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2198,13 +2198,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>3833.000</v>
+        <v>3773.000</v>
       </c>
       <c r="G58" t="s">
         <v>118</v>
       </c>
       <c r="H58" s="3">
-        <v>5747.75</v>
+        <v>5657.78</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2250,13 +2250,13 @@
         <v>122</v>
       </c>
       <c r="F60" s="2">
-        <v>163.000</v>
+        <v>161.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>31188.23</v>
+        <v>30805.55</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2770,13 +2770,13 @@
         <v>163</v>
       </c>
       <c r="F80" s="2">
-        <v>5437.500</v>
+        <v>5436.500</v>
       </c>
       <c r="G80" t="s">
         <v>157</v>
       </c>
       <c r="H80" s="3">
-        <v>12341.43</v>
+        <v>12339.15</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2822,13 +2822,13 @@
         <v>167</v>
       </c>
       <c r="F82" s="2">
-        <v>381.850</v>
+        <v>354.850</v>
       </c>
       <c r="G82" t="s">
         <v>157</v>
       </c>
       <c r="H82" s="3">
-        <v>3900.52</v>
+        <v>3624.73</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2952,13 +2952,13 @@
         <v>177</v>
       </c>
       <c r="F87" s="2">
-        <v>999.000</v>
+        <v>998.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>2507.84</v>
+        <v>2505.33</v>
       </c>
     </row>
     <row r="88" spans="1:8">

</xml_diff>

<commit_message>
#feat: escopo de materiais na familia de hidrometro, obs: falta catalogar todos os tipos de hidrometros e suas matriculas
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="216">
   <si>
     <t>4600056089</t>
   </si>
@@ -73,6 +73,12 @@
     <t>ADAPTADOR FF PPVC X BFF DN 75 X DN 80</t>
   </si>
   <si>
+    <t>30002352</t>
+  </si>
+  <si>
+    <t>CAP ELETROF - DE 63 - SDR 11 - PE 100</t>
+  </si>
+  <si>
     <t>30004405</t>
   </si>
   <si>
@@ -121,6 +127,18 @@
     <t>COLAR TOMADA ACO INOX DN50A150 X DNR20</t>
   </si>
   <si>
+    <t>30004732</t>
+  </si>
+  <si>
+    <t>COLARINHO DE 110 LG C/ FL SDR 11 PN10</t>
+  </si>
+  <si>
+    <t>30000249</t>
+  </si>
+  <si>
+    <t>COLARINHO DE 63 LG C/ FL SDR 11 PE100</t>
+  </si>
+  <si>
     <t>30004556</t>
   </si>
   <si>
@@ -307,6 +325,12 @@
     <t>LUVA CORRER BB ESG DN 100 - JE</t>
   </si>
   <si>
+    <t>30002797</t>
+  </si>
+  <si>
+    <t>LUVA CORRER BB ESG DN 100 - JEI</t>
+  </si>
+  <si>
     <t>30001548</t>
   </si>
   <si>
@@ -385,6 +409,12 @@
     <t>LUVA FF PARA PVC - EN 12842 DN 75</t>
   </si>
   <si>
+    <t>30001590</t>
+  </si>
+  <si>
+    <t>REDUCAO CONC ELETROF - DE 110 X 63</t>
+  </si>
+  <si>
     <t>30006747</t>
   </si>
   <si>
@@ -472,6 +502,12 @@
     <t>TE DE SERV INTEGR ART DN 75 P/ DE 20</t>
   </si>
   <si>
+    <t>30008695</t>
+  </si>
+  <si>
+    <t>TE FF DUCTIL C/BOLSAS JE DN 100 X 100</t>
+  </si>
+  <si>
     <t>30003716</t>
   </si>
   <si>
@@ -593,6 +629,12 @@
   </si>
   <si>
     <t>VALV GAV CM REV ELAST BB JE CAB PVC DN75</t>
+  </si>
+  <si>
+    <t>30007808</t>
+  </si>
+  <si>
+    <t>VALV GAV CM REV ELAST FL CAB DN 100</t>
   </si>
   <si>
     <t>Fornecedor</t>
@@ -723,7 +765,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,28 +785,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -810,13 +852,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>3069.32</v>
+        <v>5115.54</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -894,7 +936,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="3">
-        <v>4703.35</v>
+        <v>4703.34</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -914,13 +956,13 @@
         <v>15</v>
       </c>
       <c r="F7" s="2">
-        <v>1.000</v>
+        <v>11.000</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="3">
-        <v>97.58</v>
+        <v>1073.39</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -940,13 +982,13 @@
         <v>17</v>
       </c>
       <c r="F8" s="2">
-        <v>15.000</v>
+        <v>13.000</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="3">
-        <v>1419.82</v>
+        <v>1230.51</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -992,13 +1034,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="2">
-        <v>2.000</v>
+        <v>15.000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
-        <v>122.77</v>
+        <v>416.58</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1018,13 +1060,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>4.000</v>
+        <v>12.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>226.62</v>
+        <v>736.60</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1044,13 +1086,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>225.05</v>
+        <v>226.62</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1070,13 +1112,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2">
-        <v>10.000</v>
+        <v>5.000</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>325.39</v>
+        <v>225.05</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1096,13 +1138,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>335.45</v>
+        <v>325.39</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1128,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>62.76</v>
+        <v>335.44</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1148,13 +1190,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>1902.53</v>
+        <v>62.76</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1174,13 +1216,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>177.000</v>
+        <v>12.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>98903.17</v>
+        <v>1902.53</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1200,13 +1242,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>1.000</v>
+        <v>177.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>257.83</v>
+        <v>98903.17</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1226,13 +1268,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="2">
-        <v>748.000</v>
+        <v>8.000</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>6816.23</v>
+        <v>1674.37</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1252,13 +1294,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>30.000</v>
+        <v>11.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>480.88</v>
+        <v>1083.75</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1278,13 +1320,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>680.000</v>
+        <v>1.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>7006.06</v>
+        <v>257.83</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1304,13 +1346,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>2.000</v>
+        <v>742.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>246.82</v>
+        <v>6761.56</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1330,13 +1372,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>5.000</v>
+        <v>30.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>281.92</v>
+        <v>480.88</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1356,13 +1398,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>4.000</v>
+        <v>678.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>278.39</v>
+        <v>6970.96</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1382,13 +1424,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>130.63</v>
+        <v>246.82</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1408,13 +1450,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>40.000</v>
+        <v>5.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>207.94</v>
+        <v>281.92</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1434,13 +1476,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>13.000</v>
+        <v>4.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>1631.09</v>
+        <v>278.39</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1460,13 +1502,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>47.000</v>
+        <v>5.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>920.77</v>
+        <v>130.63</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1486,13 +1528,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>3.000</v>
+        <v>190.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>170.34</v>
+        <v>987.70</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1512,13 +1554,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>4.000</v>
+        <v>13.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>229.34</v>
+        <v>1631.09</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1538,13 +1580,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>182.000</v>
+        <v>47.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>1129.31</v>
+        <v>920.77</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1564,13 +1606,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>50.000</v>
+        <v>9.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>545.23</v>
+        <v>511.02</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1590,13 +1632,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>1878.000</v>
+        <v>4.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>48917.95</v>
+        <v>229.34</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1616,13 +1658,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>1.000</v>
+        <v>182.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>112.33</v>
+        <v>1129.31</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1642,13 +1684,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>328.000</v>
+        <v>50.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>27870.81</v>
+        <v>545.23</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1668,13 +1710,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>827.000</v>
+        <v>1797.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>113915.11</v>
+        <v>46808.01</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1694,13 +1736,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>1412.53</v>
+        <v>112.33</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1720,13 +1762,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>97.000</v>
+        <v>325.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>3599.75</v>
+        <v>27615.89</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1746,13 +1788,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>44.000</v>
+        <v>730.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>2876.22</v>
+        <v>100553.85</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1772,13 +1814,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>99.000</v>
+        <v>4.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>3261.74</v>
+        <v>1412.53</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1798,13 +1840,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>45.000</v>
+        <v>97.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>1519.40</v>
+        <v>3599.75</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1824,13 +1866,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>2842.000</v>
+        <v>44.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>10986.49</v>
+        <v>2876.22</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1850,13 +1892,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>2.000</v>
+        <v>99.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>2173.68</v>
+        <v>3261.74</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1876,13 +1918,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>6.000</v>
+        <v>45.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>10582.47</v>
+        <v>1519.40</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1902,13 +1944,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>5.000</v>
+        <v>2576.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>10490.44</v>
+        <v>9957.90</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1928,13 +1970,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>1650.27</v>
+        <v>2173.68</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1954,13 +1996,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>10.000</v>
+        <v>6.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>14423.65</v>
+        <v>10582.47</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1980,13 +2022,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>346.000</v>
+        <v>5.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>1958.64</v>
+        <v>10490.44</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2006,13 +2048,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>49.000</v>
+        <v>4.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>768.22</v>
+        <v>1650.27</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2032,13 +2074,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>49.000</v>
+        <v>10.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>1495.62</v>
+        <v>14423.65</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2058,13 +2100,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>4.000</v>
+        <v>346.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>499.92</v>
+        <v>1958.64</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2084,13 +2126,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>4.000</v>
+        <v>15.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>608.92</v>
+        <v>118.04</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2110,13 +2152,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>3.000</v>
+        <v>79.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>1417.19</v>
+        <v>1238.56</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2136,13 +2178,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>7.000</v>
+        <v>49.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>1916.14</v>
+        <v>1495.62</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2162,13 +2204,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>1480.51</v>
+        <v>499.92</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2194,7 +2236,7 @@
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>80.29</v>
+        <v>608.92</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2214,13 +2256,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>10.000</v>
+        <v>3.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>163.90</v>
+        <v>1417.19</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2240,13 +2282,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>4.000</v>
+        <v>7.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>149.66</v>
+        <v>1916.15</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2266,13 +2308,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>2.000</v>
+        <v>5.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>68.05</v>
+        <v>1480.51</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2292,13 +2334,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>41.000</v>
+        <v>4.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>4188.80</v>
+        <v>80.29</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2318,13 +2360,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>50.000</v>
+        <v>10.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>6675.45</v>
+        <v>163.90</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2344,13 +2386,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>552.000</v>
+        <v>4.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>10336.20</v>
+        <v>149.66</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2370,13 +2412,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>55.000</v>
+        <v>2.000</v>
       </c>
       <c r="G63" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>82.60</v>
+        <v>68.05</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2390,19 +2432,19 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E64" t="s">
         <v>129</v>
       </c>
-      <c r="E64" t="s">
-        <v>130</v>
-      </c>
       <c r="F64" s="2">
-        <v>12.000</v>
+        <v>61.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>427.73</v>
+        <v>6232.12</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2416,19 +2458,19 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65" t="s">
         <v>131</v>
       </c>
-      <c r="E65" t="s">
-        <v>132</v>
-      </c>
       <c r="F65" s="2">
-        <v>173.000</v>
+        <v>50.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>33101.60</v>
+        <v>6675.44</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2442,19 +2484,19 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
+        <v>132</v>
+      </c>
+      <c r="E66" t="s">
         <v>133</v>
       </c>
-      <c r="E66" t="s">
-        <v>134</v>
-      </c>
       <c r="F66" s="2">
-        <v>94.000</v>
+        <v>2.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>16414.00</v>
+        <v>120.27</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2468,19 +2510,19 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" t="s">
         <v>135</v>
       </c>
-      <c r="E67" t="s">
-        <v>136</v>
-      </c>
       <c r="F67" s="2">
-        <v>28.000</v>
+        <v>552.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>12986.24</v>
+        <v>10336.20</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2494,19 +2536,19 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68" t="s">
         <v>137</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" s="2">
+        <v>55.000</v>
+      </c>
+      <c r="G68" t="s">
         <v>138</v>
       </c>
-      <c r="F68" s="2">
-        <v>15.000</v>
-      </c>
-      <c r="G68" t="s">
-        <v>5</v>
-      </c>
       <c r="H68" s="3">
-        <v>916.05</v>
+        <v>82.72</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2526,13 +2568,13 @@
         <v>140</v>
       </c>
       <c r="F69" s="2">
-        <v>2.000</v>
+        <v>12.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>291.94</v>
+        <v>427.73</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2552,13 +2594,13 @@
         <v>142</v>
       </c>
       <c r="F70" s="2">
-        <v>10.000</v>
+        <v>185.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>104.45</v>
+        <v>35397.67</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2578,13 +2620,13 @@
         <v>144</v>
       </c>
       <c r="F71" s="2">
-        <v>2.000</v>
+        <v>130.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>195.16</v>
+        <v>22700.22</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2604,13 +2646,13 @@
         <v>146</v>
       </c>
       <c r="F72" s="2">
-        <v>1.000</v>
+        <v>48.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>207.44</v>
+        <v>22262.13</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2630,13 +2672,13 @@
         <v>148</v>
       </c>
       <c r="F73" s="2">
-        <v>79.000</v>
+        <v>35.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>2639.31</v>
+        <v>2137.45</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2656,13 +2698,13 @@
         <v>150</v>
       </c>
       <c r="F74" s="2">
-        <v>133.000</v>
+        <v>2.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>2079.10</v>
+        <v>291.93</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2682,13 +2724,13 @@
         <v>152</v>
       </c>
       <c r="F75" s="2">
-        <v>239.000</v>
+        <v>10.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>4842.14</v>
+        <v>104.45</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2714,7 +2756,7 @@
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>173.47</v>
+        <v>195.16</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2734,13 +2776,13 @@
         <v>156</v>
       </c>
       <c r="F77" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>275.49</v>
+        <v>207.44</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2760,13 +2802,13 @@
         <v>158</v>
       </c>
       <c r="F78" s="2">
-        <v>5.000</v>
+        <v>79.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>82.52</v>
+        <v>2639.31</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2786,13 +2828,13 @@
         <v>160</v>
       </c>
       <c r="F79" s="2">
-        <v>5.000</v>
+        <v>133.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>190.00</v>
+        <v>2079.10</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2812,13 +2854,13 @@
         <v>162</v>
       </c>
       <c r="F80" s="2">
-        <v>5.000</v>
+        <v>239.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>196.05</v>
+        <v>4842.14</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2844,7 +2886,7 @@
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>725.39</v>
+        <v>174.23</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2864,13 +2906,13 @@
         <v>166</v>
       </c>
       <c r="F82" s="2">
-        <v>60.000</v>
+        <v>2.000</v>
       </c>
       <c r="G82" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>2080.66</v>
+        <v>173.47</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2884,19 +2926,19 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
+        <v>167</v>
+      </c>
+      <c r="E83" t="s">
         <v>168</v>
       </c>
-      <c r="E83" t="s">
-        <v>169</v>
-      </c>
       <c r="F83" s="2">
-        <v>111.900</v>
+        <v>2.000</v>
       </c>
       <c r="G83" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>1121.25</v>
+        <v>275.49</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2910,19 +2952,19 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" t="s">
         <v>170</v>
       </c>
-      <c r="E84" t="s">
-        <v>171</v>
-      </c>
       <c r="F84" s="2">
-        <v>57.560</v>
+        <v>5.000</v>
       </c>
       <c r="G84" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>1245.48</v>
+        <v>82.52</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2936,19 +2978,19 @@
         <v>2</v>
       </c>
       <c r="D85" t="s">
+        <v>171</v>
+      </c>
+      <c r="E85" t="s">
         <v>172</v>
       </c>
-      <c r="E85" t="s">
-        <v>173</v>
-      </c>
       <c r="F85" s="2">
-        <v>7082.500</v>
+        <v>5.000</v>
       </c>
       <c r="G85" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>16074.98</v>
+        <v>190.00</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2962,19 +3004,19 @@
         <v>2</v>
       </c>
       <c r="D86" t="s">
+        <v>173</v>
+      </c>
+      <c r="E86" t="s">
         <v>174</v>
       </c>
-      <c r="E86" t="s">
-        <v>175</v>
-      </c>
       <c r="F86" s="2">
-        <v>219.850</v>
+        <v>5.000</v>
       </c>
       <c r="G86" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>938.56</v>
+        <v>196.05</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2988,19 +3030,19 @@
         <v>2</v>
       </c>
       <c r="D87" t="s">
+        <v>175</v>
+      </c>
+      <c r="E87" t="s">
         <v>176</v>
       </c>
-      <c r="E87" t="s">
-        <v>177</v>
-      </c>
       <c r="F87" s="2">
-        <v>885.850</v>
+        <v>2.000</v>
       </c>
       <c r="G87" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>9038.98</v>
+        <v>725.39</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -3014,19 +3056,19 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
+        <v>177</v>
+      </c>
+      <c r="E88" t="s">
         <v>178</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" s="2">
+        <v>60.000</v>
+      </c>
+      <c r="G88" t="s">
         <v>179</v>
       </c>
-      <c r="F88" s="2">
-        <v>299.210</v>
-      </c>
-      <c r="G88" t="s">
-        <v>167</v>
-      </c>
       <c r="H88" s="3">
-        <v>6698.90</v>
+        <v>2080.66</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3046,13 +3088,13 @@
         <v>181</v>
       </c>
       <c r="F89" s="2">
-        <v>322.490</v>
+        <v>111.900</v>
       </c>
       <c r="G89" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="H89" s="3">
-        <v>10131.49</v>
+        <v>1121.25</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3072,13 +3114,13 @@
         <v>183</v>
       </c>
       <c r="F90" s="2">
-        <v>36.000</v>
+        <v>57.560</v>
       </c>
       <c r="G90" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="H90" s="3">
-        <v>3303.06</v>
+        <v>1245.48</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3098,13 +3140,13 @@
         <v>185</v>
       </c>
       <c r="F91" s="2">
-        <v>102.430</v>
+        <v>9573.500</v>
       </c>
       <c r="G91" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="H91" s="3">
-        <v>3396.58</v>
+        <v>21728.73</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3124,13 +3166,13 @@
         <v>187</v>
       </c>
       <c r="F92" s="2">
-        <v>34.000</v>
+        <v>219.850</v>
       </c>
       <c r="G92" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="H92" s="3">
-        <v>199.07</v>
+        <v>938.56</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3150,13 +3192,13 @@
         <v>189</v>
       </c>
       <c r="F93" s="2">
-        <v>1484.000</v>
+        <v>885.850</v>
       </c>
       <c r="G93" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="H93" s="3">
-        <v>3725.36</v>
+        <v>9038.99</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3176,13 +3218,13 @@
         <v>191</v>
       </c>
       <c r="F94" s="2">
-        <v>15.000</v>
+        <v>311.210</v>
       </c>
       <c r="G94" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="H94" s="3">
-        <v>4235.73</v>
+        <v>6967.56</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3202,13 +3244,195 @@
         <v>193</v>
       </c>
       <c r="F95" s="2">
+        <v>502.490</v>
+      </c>
+      <c r="G95" t="s">
+        <v>179</v>
+      </c>
+      <c r="H95" s="3">
+        <v>15786.45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D96" t="s">
+        <v>194</v>
+      </c>
+      <c r="E96" t="s">
+        <v>195</v>
+      </c>
+      <c r="F96" s="2">
+        <v>36.000</v>
+      </c>
+      <c r="G96" t="s">
+        <v>179</v>
+      </c>
+      <c r="H96" s="3">
+        <v>3303.06</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>196</v>
+      </c>
+      <c r="E97" t="s">
+        <v>197</v>
+      </c>
+      <c r="F97" s="2">
+        <v>102.430</v>
+      </c>
+      <c r="G97" t="s">
+        <v>179</v>
+      </c>
+      <c r="H97" s="3">
+        <v>3396.58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>198</v>
+      </c>
+      <c r="E98" t="s">
+        <v>199</v>
+      </c>
+      <c r="F98" s="2">
+        <v>34.000</v>
+      </c>
+      <c r="G98" t="s">
+        <v>5</v>
+      </c>
+      <c r="H98" s="3">
+        <v>199.07</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>200</v>
+      </c>
+      <c r="E99" t="s">
+        <v>201</v>
+      </c>
+      <c r="F99" s="2">
+        <v>1832.000</v>
+      </c>
+      <c r="G99" t="s">
+        <v>5</v>
+      </c>
+      <c r="H99" s="3">
+        <v>4598.96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>202</v>
+      </c>
+      <c r="E100" t="s">
+        <v>203</v>
+      </c>
+      <c r="F100" s="2">
+        <v>15.000</v>
+      </c>
+      <c r="G100" t="s">
+        <v>5</v>
+      </c>
+      <c r="H100" s="3">
+        <v>4235.73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>204</v>
+      </c>
+      <c r="E101" t="s">
+        <v>205</v>
+      </c>
+      <c r="F101" s="2">
+        <v>13.000</v>
+      </c>
+      <c r="G101" t="s">
+        <v>5</v>
+      </c>
+      <c r="H101" s="3">
+        <v>6008.53</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>206</v>
+      </c>
+      <c r="E102" t="s">
+        <v>207</v>
+      </c>
+      <c r="F102" s="2">
         <v>7.000</v>
       </c>
-      <c r="G95" t="s">
-        <v>5</v>
-      </c>
-      <c r="H95" s="3">
-        <v>3235.36</v>
+      <c r="G102" t="s">
+        <v>5</v>
+      </c>
+      <c r="H102" s="3">
+        <v>3963.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#feat: inital refactor for hidrometro
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -1248,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>98903.17</v>
+        <v>98903.18</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1352,7 +1352,7 @@
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>6761.56</v>
+        <v>6748.24</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1404,7 +1404,7 @@
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>6970.96</v>
+        <v>6970.97</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1710,13 +1710,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>1797.000</v>
+        <v>1779.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>46808.01</v>
+        <v>46339.13</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1762,13 +1762,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>325.000</v>
+        <v>320.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>27615.89</v>
+        <v>27191.03</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1788,13 +1788,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>730.000</v>
+        <v>706.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>100553.85</v>
+        <v>97247.97</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1944,13 +1944,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>2576.000</v>
+        <v>2526.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>9957.90</v>
+        <v>9764.55</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2600,7 +2600,7 @@
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>35397.67</v>
+        <v>35397.66</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2652,7 +2652,7 @@
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>22262.13</v>
+        <v>22265.59</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3140,13 +3140,13 @@
         <v>185</v>
       </c>
       <c r="F91" s="2">
-        <v>9573.500</v>
+        <v>9560.000</v>
       </c>
       <c r="G91" t="s">
         <v>179</v>
       </c>
       <c r="H91" s="3">
-        <v>21728.73</v>
+        <v>21698.08</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3172,7 +3172,7 @@
         <v>179</v>
       </c>
       <c r="H92" s="3">
-        <v>938.56</v>
+        <v>938.55</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3348,13 +3348,13 @@
         <v>201</v>
       </c>
       <c r="F99" s="2">
-        <v>1832.000</v>
+        <v>1825.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>4598.96</v>
+        <v>4581.39</v>
       </c>
     </row>
     <row r="100" spans="1:8">

</xml_diff>

<commit_message>
Cleaning and add type annotations
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="240">
   <si>
     <t>4600056089</t>
   </si>
@@ -43,6 +43,12 @@
     <t>ABRACADEIR FF REPARO TUBO DN250 LMIN=350</t>
   </si>
   <si>
+    <t>30000255</t>
+  </si>
+  <si>
+    <t>ABRACADEIR FF REPARO TUBO DN400 LMIN=420</t>
+  </si>
+  <si>
     <t>30004091</t>
   </si>
   <si>
@@ -55,6 +61,12 @@
     <t>ABRACADEIRA FF REPARO TUBO DN75 LMIN=150</t>
   </si>
   <si>
+    <t>30008113</t>
+  </si>
+  <si>
+    <t>ADAPT PVC PPVC X BFF REKA DN 75 X 75</t>
+  </si>
+  <si>
     <t>30004242</t>
   </si>
   <si>
@@ -163,6 +175,12 @@
     <t>CONEXOES MET LIGACOES  FÊMEA DN 20</t>
   </si>
   <si>
+    <t>30001369</t>
+  </si>
+  <si>
+    <t>CRUZETA FF DUCTIL BOLSAS JE2GS DN100X100</t>
+  </si>
+  <si>
     <t>30005264</t>
   </si>
   <si>
@@ -235,6 +253,12 @@
     <t>DISPOSITIVO MED PLASTICO DN 20</t>
   </si>
   <si>
+    <t>30005517</t>
+  </si>
+  <si>
+    <t>EXTREMIDADE FF P FLG DN100 PN10/16 L=360</t>
+  </si>
+  <si>
     <t>30005519</t>
   </si>
   <si>
@@ -337,6 +361,12 @@
     <t>LUVA CORRER BB ESG DN 150 - JEI</t>
   </si>
   <si>
+    <t>30005896</t>
+  </si>
+  <si>
+    <t>LUVA CORRER BB ESG DN 200 - JE</t>
+  </si>
+  <si>
     <t>30002798</t>
   </si>
   <si>
@@ -349,6 +379,12 @@
     <t>LUVA CORRER BB ESG DN 300 - JEI</t>
   </si>
   <si>
+    <t>30002803</t>
+  </si>
+  <si>
+    <t>LUVA CORRER FF BOLSAS JE2GS DN150</t>
+  </si>
+  <si>
     <t>30005917</t>
   </si>
   <si>
@@ -391,6 +427,12 @@
     <t>LUVA ELETROF - DE 160 - SDR 11 - PE 100</t>
   </si>
   <si>
+    <t>30005752</t>
+  </si>
+  <si>
+    <t>LUVA ELETROF - DE 63 - SDR 11 - PE 100</t>
+  </si>
+  <si>
     <t>30002826</t>
   </si>
   <si>
@@ -415,6 +457,12 @@
     <t>REDUCAO CONC ELETROF - DE 110 X 63</t>
   </si>
   <si>
+    <t>30006911</t>
+  </si>
+  <si>
+    <t>REDUCAO FF PONTA BOLSA JE2GS DN100 X 75</t>
+  </si>
+  <si>
     <t>30006747</t>
   </si>
   <si>
@@ -487,7 +535,7 @@
     <t>30000211</t>
   </si>
   <si>
-    <t>TE DE SERV INTEGR ART DN 100 P/ DE 20</t>
+    <t>TE DE SERV INTEGR ART DN 100-DE 110 X 20</t>
   </si>
   <si>
     <t>30007034</t>
@@ -508,6 +556,12 @@
     <t>TE FF DUCTIL C/BOLSAS JE DN 100 X 100</t>
   </si>
   <si>
+    <t>30007286</t>
+  </si>
+  <si>
+    <t>TE FF DUCTIL C/BOLSAS JE DN 150 X 75</t>
+  </si>
+  <si>
     <t>30003716</t>
   </si>
   <si>
@@ -526,6 +580,12 @@
     <t>TE PVC BBB JE ESG DN 100 X 100 JEI</t>
   </si>
   <si>
+    <t>30007203</t>
+  </si>
+  <si>
+    <t>TE PVC BBB JE ESG DN 150 X 100- JEI/JERI</t>
+  </si>
+  <si>
     <t>30001925</t>
   </si>
   <si>
@@ -544,15 +604,21 @@
     <t>TE RED. ELETROF DE 160 X 110 PE 100</t>
   </si>
   <si>
+    <t>30007853</t>
+  </si>
+  <si>
+    <t>TUBO FF K9 PT E B JE EN 681-1 AGUA DN100</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>30028866</t>
   </si>
   <si>
     <t>TUBO PBA DN 100 1,00 MPA JEI/JERI CM 6M</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>30028862</t>
   </si>
   <si>
@@ -599,6 +665,12 @@
   </si>
   <si>
     <t>TUBO PVC RIG JEI/JERI ESG DN 300 CM 6M</t>
+  </si>
+  <si>
+    <t>30028892</t>
+  </si>
+  <si>
+    <t>TUBO PVC RIG JEI/JERI ESG DN 400 CM 6M</t>
   </si>
   <si>
     <t>30000879</t>
@@ -765,7 +837,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,28 +857,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -904,13 +976,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="3">
-        <v>767.76</v>
+        <v>4581.87</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -930,13 +1002,13 @@
         <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>11.000</v>
+        <v>8.000</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="3">
-        <v>4703.34</v>
+        <v>2047.35</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -956,13 +1028,13 @@
         <v>15</v>
       </c>
       <c r="F7" s="2">
-        <v>11.000</v>
+        <v>24.000</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="3">
-        <v>1073.39</v>
+        <v>10261.86</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -982,13 +1054,13 @@
         <v>17</v>
       </c>
       <c r="F8" s="2">
-        <v>13.000</v>
+        <v>4.000</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="3">
-        <v>1230.51</v>
+        <v>83.71</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1008,13 +1080,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>14.000</v>
+        <v>11.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>545.40</v>
+        <v>1073.39</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1034,13 +1106,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="2">
-        <v>15.000</v>
+        <v>13.000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
-        <v>416.58</v>
+        <v>1230.51</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1060,13 +1132,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>12.000</v>
+        <v>14.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>736.60</v>
+        <v>545.40</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1086,13 +1158,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>4.000</v>
+        <v>15.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>226.62</v>
+        <v>416.58</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1112,13 +1184,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2">
-        <v>5.000</v>
+        <v>12.000</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>225.05</v>
+        <v>736.60</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1138,13 +1210,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>10.000</v>
+        <v>4.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>325.39</v>
+        <v>230.24</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1164,13 +1236,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="2">
-        <v>6.000</v>
+        <v>5.000</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>335.44</v>
+        <v>225.05</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1190,13 +1262,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>62.76</v>
+        <v>325.39</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1216,13 +1288,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>1902.53</v>
+        <v>335.44</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1242,13 +1314,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>177.000</v>
+        <v>6.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>98903.18</v>
+        <v>62.76</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1268,13 +1340,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="2">
-        <v>8.000</v>
+        <v>24.000</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>1674.37</v>
+        <v>3805.08</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1294,13 +1366,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>11.000</v>
+        <v>177.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>1083.75</v>
+        <v>98903.17</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1320,13 +1392,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>257.83</v>
+        <v>1674.37</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1346,13 +1418,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>742.000</v>
+        <v>20.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>6748.24</v>
+        <v>1970.45</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1372,13 +1444,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>30.000</v>
+        <v>1.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>480.88</v>
+        <v>257.83</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1398,13 +1470,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>678.000</v>
+        <v>1107.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>6970.97</v>
+        <v>10068.08</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1424,13 +1496,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>2.000</v>
+        <v>30.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>246.82</v>
+        <v>480.88</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1450,13 +1522,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>5.000</v>
+        <v>1292.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>281.92</v>
+        <v>13284.01</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1476,13 +1548,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>278.39</v>
+        <v>215.39</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1502,13 +1574,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>130.63</v>
+        <v>246.82</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1528,13 +1600,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>190.000</v>
+        <v>5.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>987.70</v>
+        <v>281.92</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1554,13 +1626,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>13.000</v>
+        <v>4.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>1631.09</v>
+        <v>278.39</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1580,13 +1652,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>47.000</v>
+        <v>5.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>920.77</v>
+        <v>130.63</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1606,13 +1678,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>9.000</v>
+        <v>188.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>511.02</v>
+        <v>957.04</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1632,13 +1704,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>4.000</v>
+        <v>13.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>229.34</v>
+        <v>1631.09</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1658,13 +1730,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>182.000</v>
+        <v>46.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>1129.31</v>
+        <v>901.18</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1684,13 +1756,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>50.000</v>
+        <v>7.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>545.23</v>
+        <v>397.46</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1710,13 +1782,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>1779.000</v>
+        <v>4.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>46339.13</v>
+        <v>229.34</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1736,13 +1808,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>1.000</v>
+        <v>182.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>112.33</v>
+        <v>1118.70</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1762,13 +1834,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>320.000</v>
+        <v>50.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>27191.03</v>
+        <v>545.23</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1788,13 +1860,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>706.000</v>
+        <v>1911.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>97247.97</v>
+        <v>49777.24</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1814,13 +1886,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>1412.53</v>
+        <v>185.54</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1840,13 +1912,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>97.000</v>
+        <v>1.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>3599.75</v>
+        <v>112.33</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1866,13 +1938,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>44.000</v>
+        <v>633.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>2876.22</v>
+        <v>53787.37</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1892,13 +1964,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>99.000</v>
+        <v>525.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>3261.74</v>
+        <v>72316.13</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1918,13 +1990,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>45.000</v>
+        <v>4.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>1519.40</v>
+        <v>1412.53</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1944,13 +2016,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>2526.000</v>
+        <v>156.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>9764.55</v>
+        <v>5789.29</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1970,13 +2042,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>2.000</v>
+        <v>91.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>2173.68</v>
+        <v>5948.55</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1996,13 +2068,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>6.000</v>
+        <v>106.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>10582.47</v>
+        <v>3492.36</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2022,13 +2094,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>5.000</v>
+        <v>44.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>10490.44</v>
+        <v>1485.64</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2048,13 +2120,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>4.000</v>
+        <v>3512.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>1650.27</v>
+        <v>13632.34</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2074,13 +2146,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>10.000</v>
+        <v>2.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>14423.65</v>
+        <v>2173.68</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2100,13 +2172,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>346.000</v>
+        <v>8.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>1958.64</v>
+        <v>14109.96</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2126,13 +2198,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>15.000</v>
+        <v>5.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>118.04</v>
+        <v>10490.44</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2152,13 +2224,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>79.000</v>
+        <v>4.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>1238.56</v>
+        <v>1650.27</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2178,13 +2250,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>49.000</v>
+        <v>10.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>1495.62</v>
+        <v>14423.65</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2204,13 +2276,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>4.000</v>
+        <v>346.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>499.92</v>
+        <v>1958.64</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2230,13 +2302,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>4.000</v>
+        <v>9.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>608.92</v>
+        <v>74.00</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2256,13 +2328,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3.000</v>
+        <v>77.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>1417.19</v>
+        <v>1207.20</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2282,13 +2354,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>7.000</v>
+        <v>30.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>1916.15</v>
+        <v>409.01</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2308,13 +2380,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>5.000</v>
+        <v>49.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>1480.51</v>
+        <v>1495.62</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2340,7 +2412,7 @@
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>80.29</v>
+        <v>499.92</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2360,13 +2432,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>10.000</v>
+        <v>4.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>163.90</v>
+        <v>826.70</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2386,13 +2458,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>4.000</v>
+        <v>11.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>149.66</v>
+        <v>1674.52</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2412,13 +2484,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>68.05</v>
+        <v>1417.85</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2438,13 +2510,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>61.000</v>
+        <v>7.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>6232.12</v>
+        <v>1916.14</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2464,13 +2536,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>50.000</v>
+        <v>5.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>6675.44</v>
+        <v>1480.51</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2490,13 +2562,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>2.000</v>
+        <v>24.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>120.27</v>
+        <v>481.74</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2516,13 +2588,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>552.000</v>
+        <v>10.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>10336.20</v>
+        <v>163.90</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2542,13 +2614,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>55.000</v>
+        <v>4.000</v>
       </c>
       <c r="G68" t="s">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>82.72</v>
+        <v>149.66</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2562,19 +2634,19 @@
         <v>2</v>
       </c>
       <c r="D69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" t="s">
         <v>139</v>
       </c>
-      <c r="E69" t="s">
-        <v>140</v>
-      </c>
       <c r="F69" s="2">
-        <v>12.000</v>
+        <v>10.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>427.73</v>
+        <v>152.58</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2588,19 +2660,19 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
+        <v>140</v>
+      </c>
+      <c r="E70" t="s">
         <v>141</v>
       </c>
-      <c r="E70" t="s">
-        <v>142</v>
-      </c>
       <c r="F70" s="2">
-        <v>185.000</v>
+        <v>2.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>35397.66</v>
+        <v>68.05</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2614,19 +2686,19 @@
         <v>2</v>
       </c>
       <c r="D71" t="s">
+        <v>142</v>
+      </c>
+      <c r="E71" t="s">
         <v>143</v>
       </c>
-      <c r="E71" t="s">
-        <v>144</v>
-      </c>
       <c r="F71" s="2">
-        <v>130.000</v>
+        <v>61.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>22700.22</v>
+        <v>6232.12</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2640,19 +2712,19 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
+        <v>144</v>
+      </c>
+      <c r="E72" t="s">
         <v>145</v>
       </c>
-      <c r="E72" t="s">
-        <v>146</v>
-      </c>
       <c r="F72" s="2">
-        <v>48.000</v>
+        <v>80.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>22265.59</v>
+        <v>10680.71</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2666,19 +2738,19 @@
         <v>2</v>
       </c>
       <c r="D73" t="s">
+        <v>146</v>
+      </c>
+      <c r="E73" t="s">
         <v>147</v>
       </c>
-      <c r="E73" t="s">
-        <v>148</v>
-      </c>
       <c r="F73" s="2">
-        <v>35.000</v>
+        <v>2.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>2137.45</v>
+        <v>120.27</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2692,10 +2764,10 @@
         <v>2</v>
       </c>
       <c r="D74" t="s">
+        <v>148</v>
+      </c>
+      <c r="E74" t="s">
         <v>149</v>
-      </c>
-      <c r="E74" t="s">
-        <v>150</v>
       </c>
       <c r="F74" s="2">
         <v>2.000</v>
@@ -2704,7 +2776,7 @@
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>291.93</v>
+        <v>120.85</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2718,19 +2790,19 @@
         <v>2</v>
       </c>
       <c r="D75" t="s">
+        <v>150</v>
+      </c>
+      <c r="E75" t="s">
         <v>151</v>
       </c>
-      <c r="E75" t="s">
-        <v>152</v>
-      </c>
       <c r="F75" s="2">
-        <v>10.000</v>
+        <v>550.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>104.45</v>
+        <v>10298.75</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2744,19 +2816,19 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" t="s">
         <v>153</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" s="2">
+        <v>27475.000</v>
+      </c>
+      <c r="G76" t="s">
         <v>154</v>
       </c>
-      <c r="F76" s="2">
-        <v>2.000</v>
-      </c>
-      <c r="G76" t="s">
-        <v>5</v>
-      </c>
       <c r="H76" s="3">
-        <v>195.16</v>
+        <v>41527.41</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2776,13 +2848,13 @@
         <v>156</v>
       </c>
       <c r="F77" s="2">
-        <v>1.000</v>
+        <v>12.000</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>207.44</v>
+        <v>427.73</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2802,13 +2874,13 @@
         <v>158</v>
       </c>
       <c r="F78" s="2">
-        <v>79.000</v>
+        <v>204.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>2639.31</v>
+        <v>39033.08</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2828,13 +2900,13 @@
         <v>160</v>
       </c>
       <c r="F79" s="2">
-        <v>133.000</v>
+        <v>189.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>2079.10</v>
+        <v>33002.62</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2854,13 +2926,13 @@
         <v>162</v>
       </c>
       <c r="F80" s="2">
-        <v>239.000</v>
+        <v>93.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>4842.14</v>
+        <v>43139.54</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2880,13 +2952,13 @@
         <v>164</v>
       </c>
       <c r="F81" s="2">
-        <v>2.000</v>
+        <v>35.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>174.23</v>
+        <v>2137.45</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2912,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>173.47</v>
+        <v>287.19</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2932,13 +3004,13 @@
         <v>168</v>
       </c>
       <c r="F83" s="2">
-        <v>2.000</v>
+        <v>10.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>275.49</v>
+        <v>104.45</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2958,13 +3030,13 @@
         <v>170</v>
       </c>
       <c r="F84" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>82.52</v>
+        <v>195.16</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2984,13 +3056,13 @@
         <v>172</v>
       </c>
       <c r="F85" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G85" t="s">
         <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>190.00</v>
+        <v>207.44</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3010,13 +3082,13 @@
         <v>174</v>
       </c>
       <c r="F86" s="2">
-        <v>5.000</v>
+        <v>132.000</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>196.05</v>
+        <v>4409.98</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -3036,13 +3108,13 @@
         <v>176</v>
       </c>
       <c r="F87" s="2">
-        <v>2.000</v>
+        <v>133.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>725.39</v>
+        <v>2079.11</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -3062,13 +3134,13 @@
         <v>178</v>
       </c>
       <c r="F88" s="2">
-        <v>60.000</v>
+        <v>239.000</v>
       </c>
       <c r="G88" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>2080.66</v>
+        <v>4842.14</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3082,19 +3154,19 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
+        <v>179</v>
+      </c>
+      <c r="E89" t="s">
         <v>180</v>
       </c>
-      <c r="E89" t="s">
-        <v>181</v>
-      </c>
       <c r="F89" s="2">
-        <v>111.900</v>
+        <v>3.000</v>
       </c>
       <c r="G89" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>1121.25</v>
+        <v>261.34</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3108,19 +3180,19 @@
         <v>2</v>
       </c>
       <c r="D90" t="s">
+        <v>181</v>
+      </c>
+      <c r="E90" t="s">
         <v>182</v>
       </c>
-      <c r="E90" t="s">
-        <v>183</v>
-      </c>
       <c r="F90" s="2">
-        <v>57.560</v>
+        <v>2.000</v>
       </c>
       <c r="G90" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>1245.48</v>
+        <v>514.71</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3134,19 +3206,19 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
+        <v>183</v>
+      </c>
+      <c r="E91" t="s">
         <v>184</v>
       </c>
-      <c r="E91" t="s">
-        <v>185</v>
-      </c>
       <c r="F91" s="2">
-        <v>9560.000</v>
+        <v>2.000</v>
       </c>
       <c r="G91" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>21698.08</v>
+        <v>173.47</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3160,19 +3232,19 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
+        <v>185</v>
+      </c>
+      <c r="E92" t="s">
         <v>186</v>
       </c>
-      <c r="E92" t="s">
-        <v>187</v>
-      </c>
       <c r="F92" s="2">
-        <v>219.850</v>
+        <v>6.000</v>
       </c>
       <c r="G92" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>938.55</v>
+        <v>826.48</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3186,19 +3258,19 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
+        <v>187</v>
+      </c>
+      <c r="E93" t="s">
         <v>188</v>
       </c>
-      <c r="E93" t="s">
-        <v>189</v>
-      </c>
       <c r="F93" s="2">
-        <v>885.850</v>
+        <v>15.000</v>
       </c>
       <c r="G93" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>9038.99</v>
+        <v>247.55</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3212,19 +3284,19 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
+        <v>189</v>
+      </c>
+      <c r="E94" t="s">
         <v>190</v>
       </c>
-      <c r="E94" t="s">
-        <v>191</v>
-      </c>
       <c r="F94" s="2">
-        <v>311.210</v>
+        <v>1.000</v>
       </c>
       <c r="G94" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>6967.56</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3238,19 +3310,19 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
+        <v>191</v>
+      </c>
+      <c r="E95" t="s">
         <v>192</v>
       </c>
-      <c r="E95" t="s">
-        <v>193</v>
-      </c>
       <c r="F95" s="2">
-        <v>502.490</v>
+        <v>5.000</v>
       </c>
       <c r="G95" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>15786.45</v>
+        <v>190.00</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3264,19 +3336,19 @@
         <v>2</v>
       </c>
       <c r="D96" t="s">
+        <v>193</v>
+      </c>
+      <c r="E96" t="s">
         <v>194</v>
       </c>
-      <c r="E96" t="s">
-        <v>195</v>
-      </c>
       <c r="F96" s="2">
-        <v>36.000</v>
+        <v>5.000</v>
       </c>
       <c r="G96" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>3303.06</v>
+        <v>196.05</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3290,19 +3362,19 @@
         <v>2</v>
       </c>
       <c r="D97" t="s">
+        <v>195</v>
+      </c>
+      <c r="E97" t="s">
         <v>196</v>
       </c>
-      <c r="E97" t="s">
-        <v>197</v>
-      </c>
       <c r="F97" s="2">
-        <v>102.430</v>
+        <v>2.000</v>
       </c>
       <c r="G97" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>3396.58</v>
+        <v>725.39</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -3316,19 +3388,19 @@
         <v>2</v>
       </c>
       <c r="D98" t="s">
+        <v>197</v>
+      </c>
+      <c r="E98" t="s">
         <v>198</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" s="2">
+        <v>6.000</v>
+      </c>
+      <c r="G98" t="s">
         <v>199</v>
       </c>
-      <c r="F98" s="2">
-        <v>34.000</v>
-      </c>
-      <c r="G98" t="s">
-        <v>5</v>
-      </c>
       <c r="H98" s="3">
-        <v>199.07</v>
+        <v>619.70</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3348,13 +3420,13 @@
         <v>201</v>
       </c>
       <c r="F99" s="2">
-        <v>1825.000</v>
+        <v>60.000</v>
       </c>
       <c r="G99" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="H99" s="3">
-        <v>4581.39</v>
+        <v>2080.66</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -3374,13 +3446,13 @@
         <v>203</v>
       </c>
       <c r="F100" s="2">
-        <v>15.000</v>
+        <v>111.900</v>
       </c>
       <c r="G100" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="H100" s="3">
-        <v>4235.73</v>
+        <v>1121.25</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3400,13 +3472,13 @@
         <v>205</v>
       </c>
       <c r="F101" s="2">
-        <v>13.000</v>
+        <v>166.260</v>
       </c>
       <c r="G101" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="H101" s="3">
-        <v>6008.53</v>
+        <v>3597.52</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3426,12 +3498,324 @@
         <v>207</v>
       </c>
       <c r="F102" s="2">
+        <v>10694.800</v>
+      </c>
+      <c r="G102" t="s">
+        <v>199</v>
+      </c>
+      <c r="H102" s="3">
+        <v>24273.62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
+        <v>208</v>
+      </c>
+      <c r="E103" t="s">
+        <v>209</v>
+      </c>
+      <c r="F103" s="2">
+        <v>219.850</v>
+      </c>
+      <c r="G103" t="s">
+        <v>199</v>
+      </c>
+      <c r="H103" s="3">
+        <v>938.55</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>210</v>
+      </c>
+      <c r="E104" t="s">
+        <v>211</v>
+      </c>
+      <c r="F104" s="2">
+        <v>1857.850</v>
+      </c>
+      <c r="G104" t="s">
+        <v>199</v>
+      </c>
+      <c r="H104" s="3">
+        <v>18552.33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>212</v>
+      </c>
+      <c r="E105" t="s">
+        <v>213</v>
+      </c>
+      <c r="F105" s="2">
+        <v>302.210</v>
+      </c>
+      <c r="G105" t="s">
+        <v>199</v>
+      </c>
+      <c r="H105" s="3">
+        <v>6766.07</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>214</v>
+      </c>
+      <c r="E106" t="s">
+        <v>215</v>
+      </c>
+      <c r="F106" s="2">
+        <v>738.490</v>
+      </c>
+      <c r="G106" t="s">
+        <v>199</v>
+      </c>
+      <c r="H106" s="3">
+        <v>23200.74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>216</v>
+      </c>
+      <c r="E107" t="s">
+        <v>217</v>
+      </c>
+      <c r="F107" s="2">
+        <v>36.000</v>
+      </c>
+      <c r="G107" t="s">
+        <v>199</v>
+      </c>
+      <c r="H107" s="3">
+        <v>3303.06</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>218</v>
+      </c>
+      <c r="E108" t="s">
+        <v>219</v>
+      </c>
+      <c r="F108" s="2">
+        <v>6.000</v>
+      </c>
+      <c r="G108" t="s">
+        <v>199</v>
+      </c>
+      <c r="H108" s="3">
+        <v>941.24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>220</v>
+      </c>
+      <c r="E109" t="s">
+        <v>221</v>
+      </c>
+      <c r="F109" s="2">
+        <v>102.430</v>
+      </c>
+      <c r="G109" t="s">
+        <v>199</v>
+      </c>
+      <c r="H109" s="3">
+        <v>3396.58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>222</v>
+      </c>
+      <c r="E110" t="s">
+        <v>223</v>
+      </c>
+      <c r="F110" s="2">
+        <v>84.000</v>
+      </c>
+      <c r="G110" t="s">
+        <v>5</v>
+      </c>
+      <c r="H110" s="3">
+        <v>491.82</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>224</v>
+      </c>
+      <c r="E111" t="s">
+        <v>225</v>
+      </c>
+      <c r="F111" s="2">
+        <v>2257.000</v>
+      </c>
+      <c r="G111" t="s">
+        <v>5</v>
+      </c>
+      <c r="H111" s="3">
+        <v>5665.87</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" t="s">
+        <v>226</v>
+      </c>
+      <c r="E112" t="s">
+        <v>227</v>
+      </c>
+      <c r="F112" s="2">
+        <v>17.000</v>
+      </c>
+      <c r="G112" t="s">
+        <v>5</v>
+      </c>
+      <c r="H112" s="3">
+        <v>4800.49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>228</v>
+      </c>
+      <c r="E113" t="s">
+        <v>229</v>
+      </c>
+      <c r="F113" s="2">
+        <v>13.000</v>
+      </c>
+      <c r="G113" t="s">
+        <v>5</v>
+      </c>
+      <c r="H113" s="3">
+        <v>6008.53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>230</v>
+      </c>
+      <c r="E114" t="s">
+        <v>231</v>
+      </c>
+      <c r="F114" s="2">
         <v>7.000</v>
       </c>
-      <c r="G102" t="s">
-        <v>5</v>
-      </c>
-      <c r="H102" s="3">
+      <c r="G114" t="s">
+        <v>5</v>
+      </c>
+      <c r="H114" s="3">
         <v>3963.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: TROCA CV POR UMA
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -1470,13 +1470,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>1107.000</v>
+        <v>1099.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>10068.08</v>
+        <v>9995.35</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1522,13 +1522,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>1292.000</v>
+        <v>1285.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>13284.01</v>
+        <v>13212.04</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1860,13 +1860,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>1911.000</v>
+        <v>1893.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>49777.23</v>
+        <v>49308.35</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1938,13 +1938,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>631.000</v>
+        <v>630.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>53617.43</v>
+        <v>53532.46</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2120,13 +2120,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>3448.000</v>
+        <v>3283.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>13383.93</v>
+        <v>12743.48</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2822,13 +2822,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>27145.000</v>
+        <v>25705.000</v>
       </c>
       <c r="G76" t="s">
         <v>154</v>
       </c>
       <c r="H76" s="3">
-        <v>41028.63</v>
+        <v>38852.12</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3498,13 +3498,13 @@
         <v>207</v>
       </c>
       <c r="F102" s="2">
-        <v>10678.800</v>
+        <v>10620.300</v>
       </c>
       <c r="G102" t="s">
         <v>199</v>
       </c>
       <c r="H102" s="3">
-        <v>24237.30</v>
+        <v>24104.53</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3732,13 +3732,13 @@
         <v>225</v>
       </c>
       <c r="F111" s="2">
-        <v>2247.000</v>
+        <v>2219.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>5640.77</v>
+        <v>5570.48</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3764,7 +3764,7 @@
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>4800.49</v>
+        <v>4800.50</v>
       </c>
     </row>
     <row r="113" spans="1:8">

</xml_diff>

<commit_message>
#fix: return new CDispatch from rollback
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -1372,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>98903.17</v>
+        <v>98903.18</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1470,13 +1470,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>1094.000</v>
+        <v>1059.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>9949.88</v>
+        <v>9631.59</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1522,13 +1522,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>1280.000</v>
+        <v>1244.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>13160.64</v>
+        <v>12790.50</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1866,7 +1866,7 @@
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>49308.35</v>
+        <v>49308.34</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2796,13 +2796,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>549.000</v>
+        <v>533.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>10280.02</v>
+        <v>9980.43</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2822,13 +2822,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>23835.000</v>
+        <v>20604.000</v>
       </c>
       <c r="G76" t="s">
         <v>154</v>
       </c>
       <c r="H76" s="3">
-        <v>36025.69</v>
+        <v>31142.16</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3134,13 +3134,13 @@
         <v>178</v>
       </c>
       <c r="F88" s="2">
-        <v>239.000</v>
+        <v>237.000</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>4842.14</v>
+        <v>4801.62</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3498,13 +3498,13 @@
         <v>207</v>
       </c>
       <c r="F102" s="2">
-        <v>10589.800</v>
+        <v>10438.800</v>
       </c>
       <c r="G102" t="s">
         <v>199</v>
       </c>
       <c r="H102" s="3">
-        <v>24035.30</v>
+        <v>23692.57</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3732,13 +3732,13 @@
         <v>225</v>
       </c>
       <c r="F111" s="2">
-        <v>2207.000</v>
+        <v>2187.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>5540.36</v>
+        <v>5490.15</v>
       </c>
     </row>
     <row r="112" spans="1:8">

</xml_diff>

<commit_message>
add tse bloquete on lista_reposicao
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600056089.XLSX
+++ b/sheets/estoque_4600056089.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="286">
   <si>
     <t>4600056089</t>
   </si>
@@ -79,6 +79,12 @@
     <t>ADAPTADOR FF PPVC X BFF DN 100 X DN 100</t>
   </si>
   <si>
+    <t>30002028</t>
+  </si>
+  <si>
+    <t>ADAPTADOR FF PPVC X BFF DN 50 X DN 50</t>
+  </si>
+  <si>
     <t>30000518</t>
   </si>
   <si>
@@ -151,6 +157,12 @@
     <t>COLAR TOMADA ACO INOX DN50A150 X DNR20</t>
   </si>
   <si>
+    <t>30004704</t>
+  </si>
+  <si>
+    <t>COLAR TOMADA FF C.INOX DN50A150 X DNR20</t>
+  </si>
+  <si>
     <t>30002202</t>
   </si>
   <si>
@@ -169,12 +181,6 @@
     <t>COLARINHO DE 63 LG C/ FL SDR 11 PE100</t>
   </si>
   <si>
-    <t>30004556</t>
-  </si>
-  <si>
-    <t>COLARINHO DE 90 LG C/ FL SDR 11 PE 100</t>
-  </si>
-  <si>
     <t>30001346</t>
   </si>
   <si>
@@ -253,10 +259,10 @@
     <t>CURVA 90 GR PVC PB ESG DN 100 LONGA-JEI</t>
   </si>
   <si>
-    <t>30008322</t>
-  </si>
-  <si>
-    <t>CURVA 90 GR PVC PB JE ESG DN 150 LONGA</t>
+    <t>30005146</t>
+  </si>
+  <si>
+    <t>CURVA 90 GR PVC PB JE ESG DN 200</t>
   </si>
   <si>
     <t>30008324</t>
@@ -313,6 +319,12 @@
     <t>JUNTA FF BOL VAR DIA DEMAX175 X DEMIN125</t>
   </si>
   <si>
+    <t>30005604</t>
+  </si>
+  <si>
+    <t>JUNTA FF BOL VAR DIA DEMAX275 X DEMIN225</t>
+  </si>
+  <si>
     <t>30005611</t>
   </si>
   <si>
@@ -385,6 +397,12 @@
     <t>LUVA CORRER BB ESG DN 100 - JE</t>
   </si>
   <si>
+    <t>30002797</t>
+  </si>
+  <si>
+    <t>LUVA CORRER BB ESG DN 100 - JEI</t>
+  </si>
+  <si>
     <t>30005895</t>
   </si>
   <si>
@@ -517,6 +535,12 @@
     <t>REDUCAO FF PONTA BOLSA JE2GS DN100 X 75</t>
   </si>
   <si>
+    <t>30003512</t>
+  </si>
+  <si>
+    <t>REDUCAO FF PONTA BOLSA JE2GS DN80 X 75</t>
+  </si>
+  <si>
     <t>30006747</t>
   </si>
   <si>
@@ -703,6 +727,12 @@
     <t>TUBO PBA DN 75 1,00 MPA JEI/JERI CM 6M</t>
   </si>
   <si>
+    <t>30007892</t>
+  </si>
+  <si>
+    <t>TUBO PEAD AG PE 100 DE 63 PN 16</t>
+  </si>
+  <si>
     <t>30001848</t>
   </si>
   <si>
@@ -713,6 +743,12 @@
   </si>
   <si>
     <t>TUBO PEAD DN 32 - PE 80 - 1.0 MPA</t>
+  </si>
+  <si>
+    <t>30007909</t>
+  </si>
+  <si>
+    <t>TUBO PEAD PE 80 AGUA DE 90 PN12.5 SDR11</t>
   </si>
   <si>
     <t>30028856</t>
@@ -939,7 +975,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H131"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -959,28 +995,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1026,13 +1062,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="2">
-        <v>10.000</v>
+        <v>9.000</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>5115.54</v>
+        <v>4603.99</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1156,13 +1192,13 @@
         <v>17</v>
       </c>
       <c r="F8" s="2">
-        <v>8.000</v>
+        <v>7.000</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="3">
-        <v>2047.35</v>
+        <v>1791.43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1234,13 +1270,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>13.000</v>
+        <v>15.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>1230.51</v>
+        <v>571.18</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1260,13 +1296,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>14.000</v>
+        <v>11.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>545.40</v>
+        <v>1041.20</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1286,13 +1322,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2">
-        <v>15.000</v>
+        <v>29.000</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>416.58</v>
+        <v>1129.77</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1312,13 +1348,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>12.000</v>
+        <v>14.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>736.60</v>
+        <v>388.81</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1338,13 +1374,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="2">
-        <v>4.000</v>
+        <v>11.000</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>230.24</v>
+        <v>675.22</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1364,13 +1400,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>5.000</v>
+        <v>7.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>225.05</v>
+        <v>402.92</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1390,13 +1426,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>10.000</v>
+        <v>5.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>325.39</v>
+        <v>225.05</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1416,13 +1452,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>335.44</v>
+        <v>325.39</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1448,7 +1484,7 @@
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>62.76</v>
+        <v>335.44</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1468,13 +1504,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>50.000</v>
+        <v>16.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>1422.82</v>
+        <v>166.94</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1494,13 +1530,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>24.000</v>
+        <v>44.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>3805.08</v>
+        <v>1252.07</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1520,13 +1556,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>172.000</v>
+        <v>24.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>96109.30</v>
+        <v>3805.08</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1546,13 +1582,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>99.000</v>
+        <v>164.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>6237.94</v>
+        <v>91639.10</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1572,13 +1608,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>8.000</v>
+        <v>50.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>1674.37</v>
+        <v>9497.28</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1598,13 +1634,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>20.000</v>
+        <v>99.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>1970.45</v>
+        <v>6237.94</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1624,13 +1660,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>257.83</v>
+        <v>1674.37</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1650,13 +1686,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>916.000</v>
+        <v>20.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>8312.31</v>
+        <v>1970.45</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1676,13 +1712,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>30.000</v>
+        <v>1200.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>480.88</v>
+        <v>10889.70</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1702,13 +1738,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>1088.000</v>
+        <v>30.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>11182.51</v>
+        <v>480.88</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1728,13 +1764,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>1.000</v>
+        <v>1361.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>215.39</v>
+        <v>13988.34</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1754,13 +1790,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>246.82</v>
+        <v>215.39</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1780,13 +1816,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>281.93</v>
+        <v>246.82</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1806,13 +1842,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>278.39</v>
+        <v>281.93</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1832,13 +1868,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>130.63</v>
+        <v>278.39</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1858,13 +1894,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>19.000</v>
+        <v>5.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>565.15</v>
+        <v>130.63</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1884,13 +1920,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>384.000</v>
+        <v>19.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>1954.84</v>
+        <v>565.15</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1910,13 +1946,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>6.000</v>
+        <v>584.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>671.72</v>
+        <v>2973.00</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1936,13 +1972,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>13.000</v>
+        <v>6.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>1932.71</v>
+        <v>671.72</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1962,13 +1998,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>35.000</v>
+        <v>9.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>685.68</v>
+        <v>1338.03</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1988,13 +2024,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>3.000</v>
+        <v>35.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>172.00</v>
+        <v>685.68</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2014,13 +2050,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>10.000</v>
+        <v>1.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>1315.65</v>
+        <v>104.31</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2040,13 +2076,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>324.000</v>
+        <v>10.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>1991.47</v>
+        <v>1315.65</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2066,13 +2102,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>43.000</v>
+        <v>227.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>468.90</v>
+        <v>1395.20</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2092,13 +2128,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>1499.000</v>
+        <v>43.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>39045.33</v>
+        <v>468.90</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2118,13 +2154,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>1.000</v>
+        <v>1436.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>185.54</v>
+        <v>37404.20</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2150,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>112.33</v>
+        <v>185.54</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2170,13 +2206,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>1026.000</v>
+        <v>1.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>86852.76</v>
+        <v>112.33</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2196,13 +2232,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>236.000</v>
+        <v>2415.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>33187.85</v>
+        <v>204434.21</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2222,13 +2258,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>3.000</v>
+        <v>184.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>1723.63</v>
+        <v>25874.66</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2248,13 +2284,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>1412.53</v>
+        <v>3447.26</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2274,13 +2310,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>182.000</v>
+        <v>6.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>6754.17</v>
+        <v>3100.93</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2300,13 +2336,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>189.000</v>
+        <v>4.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>12354.67</v>
+        <v>1412.53</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2326,13 +2362,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>298.000</v>
+        <v>232.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>9818.10</v>
+        <v>8609.72</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2352,13 +2388,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>44.000</v>
+        <v>187.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>1485.64</v>
+        <v>12223.93</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2378,13 +2414,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>4726.000</v>
+        <v>297.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>18344.89</v>
+        <v>9785.08</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2404,13 +2440,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>2.000</v>
+        <v>44.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>2173.68</v>
+        <v>1485.64</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2430,13 +2466,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>8.000</v>
+        <v>4125.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>14109.96</v>
+        <v>16012.22</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2456,13 +2492,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>10490.44</v>
+        <v>2173.68</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2482,13 +2518,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>4.000</v>
+        <v>8.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>1650.27</v>
+        <v>14109.96</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2508,13 +2544,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>10.000</v>
+        <v>5.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>14423.65</v>
+        <v>10490.44</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2534,13 +2570,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>333.000</v>
+        <v>4.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>1885.06</v>
+        <v>1650.27</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2560,13 +2596,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>199.000</v>
+        <v>10.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>2786.00</v>
+        <v>14423.65</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2586,13 +2622,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>74.000</v>
+        <v>239.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>1160.16</v>
+        <v>1352.94</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2612,13 +2648,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>28.000</v>
+        <v>98.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>381.74</v>
+        <v>805.75</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2638,13 +2674,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>49.000</v>
+        <v>199.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>1495.62</v>
+        <v>2786.00</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2664,13 +2700,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>34.000</v>
+        <v>73.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>4249.36</v>
+        <v>1144.49</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2690,13 +2726,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>4.000</v>
+        <v>28.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>826.70</v>
+        <v>381.74</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2716,13 +2752,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>21.000</v>
+        <v>49.000</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>3196.81</v>
+        <v>1495.62</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2742,13 +2778,13 @@
         <v>139</v>
       </c>
       <c r="F69" s="2">
-        <v>9.000</v>
+        <v>34.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>4253.55</v>
+        <v>4249.36</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2768,13 +2804,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>26.000</v>
+        <v>4.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>18093.57</v>
+        <v>826.70</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2794,13 +2830,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>2.000</v>
+        <v>21.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>2320.81</v>
+        <v>3196.81</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2820,13 +2856,13 @@
         <v>145</v>
       </c>
       <c r="F72" s="2">
-        <v>20.000</v>
+        <v>9.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>6762.16</v>
+        <v>4253.55</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2846,13 +2882,13 @@
         <v>147</v>
       </c>
       <c r="F73" s="2">
-        <v>7.000</v>
+        <v>26.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>1916.14</v>
+        <v>18093.58</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2872,13 +2908,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>1480.51</v>
+        <v>2320.81</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2898,13 +2934,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>24.000</v>
+        <v>20.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>481.74</v>
+        <v>6762.16</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2924,13 +2960,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>10.000</v>
+        <v>7.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>163.90</v>
+        <v>1916.14</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2956,7 +2992,7 @@
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>149.66</v>
+        <v>1184.41</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2976,13 +3012,13 @@
         <v>157</v>
       </c>
       <c r="F78" s="2">
-        <v>10.000</v>
+        <v>24.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>152.58</v>
+        <v>481.74</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3002,13 +3038,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>22.000</v>
+        <v>6.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>748.50</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3028,13 +3064,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>61.000</v>
+        <v>4.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>6420.55</v>
+        <v>149.66</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3054,13 +3090,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>80.000</v>
+        <v>10.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>10681.36</v>
+        <v>152.58</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3080,13 +3116,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>2.000</v>
+        <v>20.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>120.27</v>
+        <v>680.45</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3106,13 +3142,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2.000</v>
+        <v>61.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>120.85</v>
+        <v>6420.55</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3132,13 +3168,13 @@
         <v>169</v>
       </c>
       <c r="F84" s="2">
-        <v>765.000</v>
+        <v>80.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>14324.62</v>
+        <v>10681.35</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3158,13 +3194,13 @@
         <v>171</v>
       </c>
       <c r="F85" s="2">
-        <v>30754.000</v>
+        <v>2.000</v>
       </c>
       <c r="G85" t="s">
-        <v>172</v>
+        <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>46621.78</v>
+        <v>120.27</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3178,19 +3214,19 @@
         <v>2</v>
       </c>
       <c r="D86" t="s">
+        <v>172</v>
+      </c>
+      <c r="E86" t="s">
         <v>173</v>
       </c>
-      <c r="E86" t="s">
-        <v>174</v>
-      </c>
       <c r="F86" s="2">
-        <v>12.000</v>
+        <v>2.000</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>427.73</v>
+        <v>120.85</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -3204,19 +3240,19 @@
         <v>2</v>
       </c>
       <c r="D87" t="s">
+        <v>174</v>
+      </c>
+      <c r="E87" t="s">
         <v>175</v>
       </c>
-      <c r="E87" t="s">
-        <v>176</v>
-      </c>
       <c r="F87" s="2">
-        <v>275.000</v>
+        <v>20.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>52618.09</v>
+        <v>696.06</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -3230,19 +3266,19 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
+        <v>176</v>
+      </c>
+      <c r="E88" t="s">
         <v>177</v>
       </c>
-      <c r="E88" t="s">
-        <v>178</v>
-      </c>
       <c r="F88" s="2">
-        <v>321.000</v>
+        <v>755.000</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>56052.04</v>
+        <v>14137.38</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3256,19 +3292,19 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
+        <v>178</v>
+      </c>
+      <c r="E89" t="s">
         <v>179</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" s="2">
+        <v>24854.000</v>
+      </c>
+      <c r="G89" t="s">
         <v>180</v>
       </c>
-      <c r="F89" s="2">
-        <v>36.000</v>
-      </c>
-      <c r="G89" t="s">
-        <v>5</v>
-      </c>
       <c r="H89" s="3">
-        <v>6081.40</v>
+        <v>37786.81</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3288,13 +3324,13 @@
         <v>182</v>
       </c>
       <c r="F90" s="2">
-        <v>149.000</v>
+        <v>12.000</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>69115.89</v>
+        <v>427.73</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3314,13 +3350,13 @@
         <v>184</v>
       </c>
       <c r="F91" s="2">
-        <v>35.000</v>
+        <v>284.000</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>2137.45</v>
+        <v>54340.13</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3340,13 +3376,13 @@
         <v>186</v>
       </c>
       <c r="F92" s="2">
-        <v>22.000</v>
+        <v>227.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>3159.63</v>
+        <v>39638.02</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -3366,13 +3402,13 @@
         <v>188</v>
       </c>
       <c r="F93" s="2">
-        <v>10.000</v>
+        <v>36.000</v>
       </c>
       <c r="G93" t="s">
         <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>104.45</v>
+        <v>6081.40</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3392,13 +3428,13 @@
         <v>190</v>
       </c>
       <c r="F94" s="2">
-        <v>2.000</v>
+        <v>146.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>195.16</v>
+        <v>67724.29</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3418,13 +3454,13 @@
         <v>192</v>
       </c>
       <c r="F95" s="2">
-        <v>1.000</v>
+        <v>35.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>207.44</v>
+        <v>2137.45</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3444,13 +3480,13 @@
         <v>194</v>
       </c>
       <c r="F96" s="2">
-        <v>132.000</v>
+        <v>22.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>4409.98</v>
+        <v>3159.63</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3470,13 +3506,13 @@
         <v>196</v>
       </c>
       <c r="F97" s="2">
-        <v>132.000</v>
+        <v>10.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>2063.49</v>
+        <v>104.45</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -3496,13 +3532,13 @@
         <v>198</v>
       </c>
       <c r="F98" s="2">
-        <v>226.000</v>
+        <v>1.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>4578.76</v>
+        <v>97.58</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3522,13 +3558,13 @@
         <v>200</v>
       </c>
       <c r="F99" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>261.34</v>
+        <v>207.44</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -3548,13 +3584,13 @@
         <v>202</v>
       </c>
       <c r="F100" s="2">
-        <v>2.000</v>
+        <v>131.000</v>
       </c>
       <c r="G100" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>514.71</v>
+        <v>4376.57</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3574,13 +3610,13 @@
         <v>204</v>
       </c>
       <c r="F101" s="2">
-        <v>2.000</v>
+        <v>132.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>173.47</v>
+        <v>2063.51</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3600,13 +3636,13 @@
         <v>206</v>
       </c>
       <c r="F102" s="2">
-        <v>5.000</v>
+        <v>212.000</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>1344.99</v>
+        <v>4295.12</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3626,13 +3662,13 @@
         <v>208</v>
       </c>
       <c r="F103" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G103" t="s">
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>649.65</v>
+        <v>261.34</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3652,13 +3688,13 @@
         <v>210</v>
       </c>
       <c r="F104" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>834.99</v>
+        <v>514.71</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3678,13 +3714,13 @@
         <v>212</v>
       </c>
       <c r="F105" s="2">
-        <v>15.000</v>
+        <v>2.000</v>
       </c>
       <c r="G105" t="s">
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>247.55</v>
+        <v>173.47</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3704,13 +3740,13 @@
         <v>214</v>
       </c>
       <c r="F106" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G106" t="s">
         <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>23.34</v>
+        <v>1344.99</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3736,7 +3772,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>190.00</v>
+        <v>649.65</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3756,13 +3792,13 @@
         <v>218</v>
       </c>
       <c r="F108" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G108" t="s">
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>196.05</v>
+        <v>834.99</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3782,13 +3818,13 @@
         <v>220</v>
       </c>
       <c r="F109" s="2">
-        <v>2.000</v>
+        <v>15.000</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>725.39</v>
+        <v>247.55</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3808,13 +3844,13 @@
         <v>222</v>
       </c>
       <c r="F110" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G110" t="s">
-        <v>223</v>
+        <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>619.70</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3828,19 +3864,19 @@
         <v>2</v>
       </c>
       <c r="D111" t="s">
+        <v>223</v>
+      </c>
+      <c r="E111" t="s">
         <v>224</v>
       </c>
-      <c r="E111" t="s">
-        <v>225</v>
-      </c>
       <c r="F111" s="2">
-        <v>60.000</v>
+        <v>5.000</v>
       </c>
       <c r="G111" t="s">
-        <v>223</v>
+        <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>2080.66</v>
+        <v>190.00</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3854,19 +3890,19 @@
         <v>2</v>
       </c>
       <c r="D112" t="s">
+        <v>225</v>
+      </c>
+      <c r="E112" t="s">
         <v>226</v>
       </c>
-      <c r="E112" t="s">
-        <v>227</v>
-      </c>
       <c r="F112" s="2">
-        <v>171.900</v>
+        <v>5.000</v>
       </c>
       <c r="G112" t="s">
-        <v>223</v>
+        <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>1722.46</v>
+        <v>196.05</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3880,19 +3916,19 @@
         <v>2</v>
       </c>
       <c r="D113" t="s">
+        <v>227</v>
+      </c>
+      <c r="E113" t="s">
         <v>228</v>
       </c>
-      <c r="E113" t="s">
-        <v>229</v>
-      </c>
       <c r="F113" s="2">
-        <v>166.260</v>
+        <v>2.000</v>
       </c>
       <c r="G113" t="s">
-        <v>223</v>
+        <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>3597.52</v>
+        <v>725.39</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3906,19 +3942,19 @@
         <v>2</v>
       </c>
       <c r="D114" t="s">
+        <v>229</v>
+      </c>
+      <c r="E114" t="s">
         <v>230</v>
       </c>
-      <c r="E114" t="s">
+      <c r="F114" s="2">
+        <v>6.000</v>
+      </c>
+      <c r="G114" t="s">
         <v>231</v>
       </c>
-      <c r="F114" s="2">
-        <v>9475.300</v>
-      </c>
-      <c r="G114" t="s">
-        <v>223</v>
-      </c>
       <c r="H114" s="3">
-        <v>21502.25</v>
+        <v>619.70</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3938,13 +3974,13 @@
         <v>233</v>
       </c>
       <c r="F115" s="2">
-        <v>1019.850</v>
+        <v>60.000</v>
       </c>
       <c r="G115" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H115" s="3">
-        <v>4475.80</v>
+        <v>2080.66</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3964,13 +4000,13 @@
         <v>235</v>
       </c>
       <c r="F116" s="2">
-        <v>2362.150</v>
+        <v>171.900</v>
       </c>
       <c r="G116" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H116" s="3">
-        <v>23572.24</v>
+        <v>1722.46</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3990,13 +4026,13 @@
         <v>237</v>
       </c>
       <c r="F117" s="2">
-        <v>706.210</v>
+        <v>158.600</v>
       </c>
       <c r="G117" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H117" s="3">
-        <v>15811.07</v>
+        <v>3431.78</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4016,13 +4052,13 @@
         <v>239</v>
       </c>
       <c r="F118" s="2">
-        <v>602.660</v>
+        <v>213.270</v>
       </c>
       <c r="G118" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H118" s="3">
-        <v>18933.44</v>
+        <v>3743.86</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4042,13 +4078,13 @@
         <v>241</v>
       </c>
       <c r="F119" s="2">
-        <v>19.150</v>
+        <v>10100.300</v>
       </c>
       <c r="G119" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H119" s="3">
-        <v>1757.05</v>
+        <v>22918.12</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4068,13 +4104,13 @@
         <v>243</v>
       </c>
       <c r="F120" s="2">
-        <v>6.000</v>
+        <v>1019.850</v>
       </c>
       <c r="G120" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H120" s="3">
-        <v>941.24</v>
+        <v>4475.80</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4094,13 +4130,13 @@
         <v>245</v>
       </c>
       <c r="F121" s="2">
-        <v>230.000</v>
+        <v>4.800</v>
       </c>
       <c r="G121" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H121" s="3">
-        <v>7433.20</v>
+        <v>180.48</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4120,13 +4156,13 @@
         <v>247</v>
       </c>
       <c r="F122" s="2">
-        <v>102.430</v>
+        <v>2022.650</v>
       </c>
       <c r="G122" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="H122" s="3">
-        <v>3396.58</v>
+        <v>20184.71</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4146,13 +4182,13 @@
         <v>249</v>
       </c>
       <c r="F123" s="2">
-        <v>82.000</v>
+        <v>686.710</v>
       </c>
       <c r="G123" t="s">
-        <v>5</v>
+        <v>231</v>
       </c>
       <c r="H123" s="3">
-        <v>480.11</v>
+        <v>15374.49</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4172,13 +4208,13 @@
         <v>251</v>
       </c>
       <c r="F124" s="2">
-        <v>24.000</v>
+        <v>485.950</v>
       </c>
       <c r="G124" t="s">
-        <v>5</v>
+        <v>231</v>
       </c>
       <c r="H124" s="3">
-        <v>132.21</v>
+        <v>15266.82</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4198,13 +4234,13 @@
         <v>253</v>
       </c>
       <c r="F125" s="2">
-        <v>2485.000</v>
+        <v>19.150</v>
       </c>
       <c r="G125" t="s">
-        <v>5</v>
+        <v>231</v>
       </c>
       <c r="H125" s="3">
-        <v>6238.25</v>
+        <v>1757.05</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -4224,13 +4260,13 @@
         <v>255</v>
       </c>
       <c r="F126" s="2">
-        <v>17.000</v>
+        <v>6.000</v>
       </c>
       <c r="G126" t="s">
-        <v>5</v>
+        <v>231</v>
       </c>
       <c r="H126" s="3">
-        <v>4800.50</v>
+        <v>941.24</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -4250,13 +4286,13 @@
         <v>257</v>
       </c>
       <c r="F127" s="2">
-        <v>13.000</v>
+        <v>230.000</v>
       </c>
       <c r="G127" t="s">
-        <v>5</v>
+        <v>231</v>
       </c>
       <c r="H127" s="3">
-        <v>6008.53</v>
+        <v>7433.20</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -4276,13 +4312,13 @@
         <v>259</v>
       </c>
       <c r="F128" s="2">
-        <v>7.000</v>
+        <v>102.430</v>
       </c>
       <c r="G128" t="s">
-        <v>5</v>
+        <v>231</v>
       </c>
       <c r="H128" s="3">
-        <v>3963.06</v>
+        <v>3396.58</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -4302,13 +4338,13 @@
         <v>261</v>
       </c>
       <c r="F129" s="2">
-        <v>5.000</v>
+        <v>82.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>1833.01</v>
+        <v>480.11</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -4328,13 +4364,13 @@
         <v>263</v>
       </c>
       <c r="F130" s="2">
-        <v>4.000</v>
+        <v>24.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>1840.82</v>
+        <v>132.21</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4354,13 +4390,169 @@
         <v>265</v>
       </c>
       <c r="F131" s="2">
+        <v>2384.000</v>
+      </c>
+      <c r="G131" t="s">
+        <v>5</v>
+      </c>
+      <c r="H131" s="3">
+        <v>5984.71</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" t="s">
+        <v>266</v>
+      </c>
+      <c r="E132" t="s">
+        <v>267</v>
+      </c>
+      <c r="F132" s="2">
+        <v>16.000</v>
+      </c>
+      <c r="G132" t="s">
+        <v>5</v>
+      </c>
+      <c r="H132" s="3">
+        <v>4518.12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" t="s">
+        <v>268</v>
+      </c>
+      <c r="E133" t="s">
+        <v>269</v>
+      </c>
+      <c r="F133" s="2">
+        <v>12.000</v>
+      </c>
+      <c r="G133" t="s">
+        <v>5</v>
+      </c>
+      <c r="H133" s="3">
+        <v>5546.33</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" t="s">
+        <v>270</v>
+      </c>
+      <c r="E134" t="s">
+        <v>271</v>
+      </c>
+      <c r="F134" s="2">
+        <v>7.000</v>
+      </c>
+      <c r="G134" t="s">
+        <v>5</v>
+      </c>
+      <c r="H134" s="3">
+        <v>3963.06</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" t="s">
+        <v>272</v>
+      </c>
+      <c r="E135" t="s">
+        <v>273</v>
+      </c>
+      <c r="F135" s="2">
+        <v>5.000</v>
+      </c>
+      <c r="G135" t="s">
+        <v>5</v>
+      </c>
+      <c r="H135" s="3">
+        <v>1833.01</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" t="s">
+        <v>274</v>
+      </c>
+      <c r="E136" t="s">
+        <v>275</v>
+      </c>
+      <c r="F136" s="2">
         <v>4.000</v>
       </c>
-      <c r="G131" t="s">
-        <v>5</v>
-      </c>
-      <c r="H131" s="3">
-        <v>2253.28</v>
+      <c r="G136" t="s">
+        <v>5</v>
+      </c>
+      <c r="H136" s="3">
+        <v>1840.82</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137" t="s">
+        <v>276</v>
+      </c>
+      <c r="E137" t="s">
+        <v>277</v>
+      </c>
+      <c r="F137" s="2">
+        <v>3.000</v>
+      </c>
+      <c r="G137" t="s">
+        <v>5</v>
+      </c>
+      <c r="H137" s="3">
+        <v>1689.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>